<commit_message>
new features to MaxTable
</commit_message>
<xml_diff>
--- a/templates/maxTemplate.xlsx
+++ b/templates/maxTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdel\OneDrive\Desktop\yazaki\xlsx git\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E129FD-314A-46A2-BE16-0CADC127A2B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B16C154-C00A-4E52-AD90-57B2AD27A994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,18 +570,18 @@
   <dimension ref="A1:BD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
@@ -635,25 +635,25 @@
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>

</xml_diff>